<commit_message>
color coded wealth brackets
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arcop\Documents\excel_git_example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1FCD998E-C0BA-467A-B364-ABEEEBF6BC0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E51DA2EA-F42A-4471-BF6F-A75F4525F4C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{393C64AD-28FA-4327-A7CC-498ECF6FBE33}"/>
   </bookViews>
@@ -57,8 +57,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -99,13 +100,44 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -418,12 +450,12 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="15.3125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.3125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -464,6 +496,14 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B3:B5">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+      <formula>99000000</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+      <formula>50000000</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added net worth graph
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arcop\Documents\excel_git_example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1FCD998E-C0BA-467A-B364-ABEEEBF6BC0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C0EC9B-25FD-4D3F-ABA1-7F8418932F59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{393C64AD-28FA-4327-A7CC-498ECF6FBE33}"/>
   </bookViews>
@@ -116,6 +116,973 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>net worth</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="&quot;$&quot;#,##0" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$3:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>farty mcfartface</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>jebediah berkely</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>young jesus</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>23000000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>583859933</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40059533</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-94B9-4EC9-BF43-2D0AA2AE9038}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1710058176"/>
+        <c:axId val="1701447840"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1710058176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1701447840"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1701447840"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="1000000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)" sourceLinked="0"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1710058176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="10"/>
+        <c:dispUnits>
+          <c:builtInUnit val="millions"/>
+          <c:dispUnitsLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>146685</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>146685</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05D0CEAB-6C9A-401B-991D-A18BBD5F1878}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -418,7 +1385,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -465,5 +1432,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
restructured brackets, added individuals
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arcop\Documents\excel_git_example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E51DA2EA-F42A-4471-BF6F-A75F4525F4C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A1B713-347C-4994-8332-9677380FFEBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{393C64AD-28FA-4327-A7CC-498ECF6FBE33}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Data on rich people</t>
   </si>
@@ -52,6 +52,12 @@
   <si>
     <t>net worth</t>
   </si>
+  <si>
+    <t>eli strumpleton</t>
+  </si>
+  <si>
+    <t>frumpf von der halen</t>
+  </si>
 </sst>
 </file>
 
@@ -59,9 +65,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,6 +76,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -98,22 +112,233 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -447,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{563BE999-E00F-4004-969F-D470347E34FD}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -459,7 +684,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
@@ -495,15 +720,51 @@
         <v>40059533</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>70000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <v>120445000</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B3:B5">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="greaterThan">
       <formula>99000000</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="lessThan">
       <formula>50000000</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B6:B7">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="lessThan">
+      <formula>50000000</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="greaterThan">
+      <formula>99000000</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:B7">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+      <formula>50000000</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+      <formula>50000000</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+      <formula>100000000</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>